<commit_message>
Updated description of classes to date in package Signed-off-by: bridroberts <brid.roberts@ucdconnect.ie>
</commit_message>
<xml_diff>
--- a/notes/ClassDescriptions.xlsx
+++ b/notes/ClassDescriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B Roberts\OneDrive - University College Dublin\5th Year\SoftwareEngineering\GameOfLife\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B2F5C2B-3F37-4677-A5EE-AE862DB71C6E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{9B2F5C2B-3F37-4677-A5EE-AE862DB71C6E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{387391B2-8C25-4222-B0D1-8A460428835C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{14451809-876C-4749-995F-25794DA69D0B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="142">
   <si>
     <t>Class</t>
   </si>
@@ -252,13 +252,217 @@
   </si>
   <si>
     <t>Player player1</t>
+  </si>
+  <si>
+    <t>Cards: Career Cards</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>CareerCards(String fileLocation)</t>
+  </si>
+  <si>
+    <t>CareerCards(String fileLocation, String name, int value1, int value2)</t>
+  </si>
+  <si>
+    <t>N/A Constructor</t>
+  </si>
+  <si>
+    <t>getValue2List(List&lt;String&gt; inputList)</t>
+  </si>
+  <si>
+    <t>getListOfCards(String fileLocation)</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;String&gt; value2List</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;CareerCards&gt; listOfCards</t>
+  </si>
+  <si>
+    <t>getValue2()</t>
+  </si>
+  <si>
+    <t>int value2</t>
+  </si>
+  <si>
+    <t>Cards: House Cards</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>HouseCards(String fileLocation)</t>
+  </si>
+  <si>
+    <t>HouseCards(String fileLocation, String name, int value1, int value2, int value3)</t>
+  </si>
+  <si>
+    <t>getValue2List(List&lt;String&gt;  inputList)</t>
+  </si>
+  <si>
+    <t>getValue3List(List&lt;String&gt; inputList)</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;String&gt; value3List</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;HouseCards&gt; listOfCards</t>
+  </si>
+  <si>
+    <t>getValue3()</t>
+  </si>
+  <si>
+    <t>int value3</t>
+  </si>
+  <si>
+    <t>Cards: Action Cards</t>
+  </si>
+  <si>
+    <t>getListOfCards()</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;String&gt; cardList</t>
+  </si>
+  <si>
+    <t>chooseActionCard(ArrayList&lt;String&gt; cardList)</t>
+  </si>
+  <si>
+    <t>Spinner</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>spin</t>
+  </si>
+  <si>
+    <t>Spinner()</t>
+  </si>
+  <si>
+    <t>spinSpinner()</t>
+  </si>
+  <si>
+    <t>getNumber()</t>
+  </si>
+  <si>
+    <t>int spin</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt;</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>Space(String number, List&lt;String&gt; type, List&lt;String&gt; next)</t>
+  </si>
+  <si>
+    <t>printSpace()</t>
+  </si>
+  <si>
+    <t>getSpaceType()</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt; type</t>
+  </si>
+  <si>
+    <t>getNextSpace()</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt; next</t>
+  </si>
+  <si>
+    <t>getNumberSpace()</t>
+  </si>
+  <si>
+    <t>String number</t>
+  </si>
+  <si>
+    <t>BoardReader</t>
+  </si>
+  <si>
+    <t>readBoard()</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Space&gt; boardSpacesList</t>
+  </si>
+  <si>
+    <t>InitialiseGame</t>
+  </si>
+  <si>
+    <t>InitialiseGame()</t>
+  </si>
+  <si>
+    <t>initialisePawns()</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Player&gt; listOfPlayers</t>
+  </si>
+  <si>
+    <t>initialiseHouseDeck()</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;HouseCards&gt; houseList</t>
+  </si>
+  <si>
+    <t>initialiseCareerCardDeck(String fileLocation)</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;CareerCards&gt; careerList</t>
+  </si>
+  <si>
+    <t>initialiseActionCardDeck()</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;String&gt; actionCardList</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>propFileName</t>
+  </si>
+  <si>
+    <t>utility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prop </t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Utility()</t>
+  </si>
+  <si>
+    <t>getProperty(String key)</t>
+  </si>
+  <si>
+    <t>getInstance()</t>
+  </si>
+  <si>
+    <t>String prop.getProperty(key)</t>
+  </si>
+  <si>
+    <t>Utility utility</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +481,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,13 +513,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CA32F8-110B-494D-B220-36515DE376B1}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,13 +846,13 @@
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -981,12 +1193,380 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>71</v>
       </c>
       <c r="E33" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>98</v>
+      </c>
+      <c r="E53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>111</v>
+      </c>
+      <c r="E61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" t="s">
+        <v>113</v>
+      </c>
+      <c r="E63" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>115</v>
+      </c>
+      <c r="E64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D67" t="s">
+        <v>120</v>
+      </c>
+      <c r="E67" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D69" t="s">
+        <v>123</v>
+      </c>
+      <c r="E69" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>124</v>
+      </c>
+      <c r="E70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>126</v>
+      </c>
+      <c r="E71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>128</v>
+      </c>
+      <c r="E72" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>130</v>
+      </c>
+      <c r="E73" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" t="s">
+        <v>137</v>
+      </c>
+      <c r="E75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>134</v>
+      </c>
+      <c r="C76" t="s">
+        <v>132</v>
+      </c>
+      <c r="D76" t="s">
+        <v>138</v>
+      </c>
+      <c r="E76" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" t="s">
+        <v>136</v>
+      </c>
+      <c r="D77" t="s">
+        <v>139</v>
+      </c>
+      <c r="E77" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ClassDescriptions excel sheet and to do document Signed-off-by: bridroberts <brid.roberts@ucdconnect.ie>
</commit_message>
<xml_diff>
--- a/notes/ClassDescriptions.xlsx
+++ b/notes/ClassDescriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B Roberts\OneDrive - University College Dublin\5th Year\SoftwareEngineering\GameOfLife\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="479" documentId="8_{9B2F5C2B-3F37-4677-A5EE-AE862DB71C6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7E36C479-FACA-4611-B5CF-2AD0FB8A49D8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D137A56A-38ED-475B-86BA-EBE1E19F3196}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{14451809-876C-4749-995F-25794DA69D0B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="331">
   <si>
     <t>Class</t>
   </si>
@@ -935,14 +935,122 @@
     <t>construct a StopSpace object</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: A team member has been assigned to each class. In some cases, there are two team members names listed. This represents paired programming sessions. </t>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF9C5700"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF9C5700"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A team member has been assigned to each class. In some cases, there are two team members names listed. This represents classes written during paired programming sessions which took place at least once a week. </t>
+    </r>
+  </si>
+  <si>
+    <t>Deck</t>
+  </si>
+  <si>
+    <t>actionCardDeck</t>
+  </si>
+  <si>
+    <t>careerCardDeck</t>
+  </si>
+  <si>
+    <t>collegeCareerCardDeck</t>
+  </si>
+  <si>
+    <t>houseCardDeck</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;ActionCards&gt;</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;CareerCards&gt;</t>
+  </si>
+  <si>
+    <t>Deck()</t>
+  </si>
+  <si>
+    <t>Deck(ArrayList&lt;ActionCards&gt; actionCardDeck, ArrayList&lt;CareerCards&gt; careerCardDeck, ArrayList&lt;CareerCards&gt; collegeCareerCardDeck, ArrayList&lt;HouseCards&gt; houseCardDeck</t>
+  </si>
+  <si>
+    <t>Deck cardDeck</t>
+  </si>
+  <si>
+    <t>construct a deck object using inputs to set attributes</t>
+  </si>
+  <si>
+    <t>construct a deck object using no inputs, here the attributes are set to null</t>
+  </si>
+  <si>
+    <t>getActionCardDeck()</t>
+  </si>
+  <si>
+    <t>getCareerCardDeck()</t>
+  </si>
+  <si>
+    <t>getCollegeCareerCardDeck()</t>
+  </si>
+  <si>
+    <t>getHouseCardDeck()</t>
+  </si>
+  <si>
+    <t>method to return a deck of ActionCard objects</t>
+  </si>
+  <si>
+    <t>method to return a deck of CareerCard objects</t>
+  </si>
+  <si>
+    <t>method to return a deck of HouseCard objects</t>
+  </si>
+  <si>
+    <t>makeBoard()</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Spaces&gt;</t>
+  </si>
+  <si>
+    <t>makeCards(Scanner keyboard)</t>
+  </si>
+  <si>
+    <t>makePlayers(ArrayList&lt;CareerCards collegeCareerCardDeck, Scanner keyboard)</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Players&gt;</t>
+  </si>
+  <si>
+    <t>playGame(Deck cardDeck, ArrayList&lt;Spaces&gt; boardSpaces,  ArrayList&lt;Players&gt; listOfPlayers, Scanner keyboard)</t>
+  </si>
+  <si>
+    <t>method to create the board using spaces detailed in a text file</t>
+  </si>
+  <si>
+    <t>method to create the card decks: action cards, career cards, college career cards and house cards</t>
+  </si>
+  <si>
+    <t>method to create an array list of initialised players</t>
+  </si>
+  <si>
+    <t>method invoked to start to play the game, play continues until all players retire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -959,14 +1067,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -974,6 +1074,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="14"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -1015,27 +1139,21 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1353,1448 +1471,1591 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CA32F8-110B-494D-B220-36515DE376B1}">
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="H135" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J144" sqref="J144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="7" width="62.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="35" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="40" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="62.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="E3" t="s">
+    <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="E4" t="s">
+    <row r="4" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+    <row r="5" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+    <row r="6" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+    <row r="7" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
+    <row r="8" spans="1:9" ht="126" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+    <row r="9" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="6" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="6" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+    <row r="13" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="6" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G14" s="4" t="s">
+    <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G15" s="4" t="s">
+    <row r="15" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G16" s="4" t="s">
+    <row r="16" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="7:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G17" s="4" t="s">
+    <row r="17" spans="7:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G17" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="6" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="7:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="G18" s="4" t="s">
+    <row r="18" spans="7:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G18" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="7:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G19" s="4" t="s">
+    <row r="19" spans="7:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G19" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="7:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G20" s="4" t="s">
+    <row r="20" spans="7:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G20" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="H20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="H20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="7:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G21" s="4" t="s">
+    <row r="21" spans="7:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G21" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H21" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" s="4" t="s">
+      <c r="H21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="7:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G22" s="4" t="s">
+    <row r="22" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G22" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="H22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" s="4" t="s">
+      <c r="H22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="7:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="G23" s="4" t="s">
+    <row r="23" spans="7:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="G23" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H23" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23" s="4" t="s">
+      <c r="H23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="7:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G24" s="4" t="s">
+    <row r="24" spans="7:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G24" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="7:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G25" s="4" t="s">
+    <row r="25" spans="7:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G25" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="7:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G26" s="4" t="s">
+    <row r="26" spans="7:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G26" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="7:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="G27" s="4" t="s">
+    <row r="27" spans="7:9" ht="126" x14ac:dyDescent="0.25">
+      <c r="G27" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="7:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G28" s="4" t="s">
+    <row r="28" spans="7:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G28" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="H28" t="s">
-        <v>32</v>
-      </c>
-      <c r="I28" s="4" t="s">
+      <c r="H28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="7:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="G29" s="4" t="s">
+    <row r="29" spans="7:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G29" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H29" t="s">
-        <v>32</v>
-      </c>
-      <c r="I29" s="4" t="s">
+      <c r="H29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="7:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="G30" s="4" t="s">
+    <row r="30" spans="7:9" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="G30" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="H30" t="s">
-        <v>32</v>
-      </c>
-      <c r="I30" s="4" t="s">
+      <c r="H30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="7:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G31" s="4" t="s">
+    <row r="31" spans="7:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G31" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I31" s="4" t="s">
+      <c r="H31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="7:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="G32" s="4" t="s">
+    <row r="32" spans="7:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="G32" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="G33" s="4" t="s">
+    <row r="33" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G33" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H33" t="s">
-        <v>32</v>
-      </c>
-      <c r="I33" s="4" t="s">
+      <c r="H33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
+    <row r="37" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
+    <row r="38" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="E38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="6" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="3:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
+    <row r="39" spans="3:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="I39" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G40" s="4" t="s">
+    <row r="40" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G40" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="6" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G41" s="4" t="s">
+    <row r="41" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G41" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" s="6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G42" s="4" t="s">
+    <row r="42" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G42" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I42" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="43" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G43" s="4" t="s">
+    <row r="43" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G43" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" s="6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="44" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G44" s="4" t="s">
+    <row r="44" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G44" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I44" s="6" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G45" s="4" t="s">
+    <row r="45" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G45" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="I45" s="6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G46" s="4" t="s">
+    <row r="46" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G46" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H46" t="s">
-        <v>32</v>
-      </c>
-      <c r="I46" s="4" t="s">
+      <c r="H46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I46" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C49" s="3" t="s">
+    <row r="49" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C49" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G49" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="I49" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G50" s="4" t="s">
+    <row r="50" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G50" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I50" s="4" t="s">
+      <c r="I50" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="G51" s="4" t="s">
+    <row r="51" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G51" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="I51" s="6" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="52" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G52" s="4" t="s">
+    <row r="52" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G52" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I52" s="4" t="s">
+      <c r="I52" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="G53" s="4" t="s">
+    <row r="53" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G53" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I53" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="54" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G54" s="4" t="s">
+    <row r="54" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G54" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H54" t="s">
-        <v>32</v>
-      </c>
-      <c r="I54" s="4" t="s">
+      <c r="H54" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I54" s="6" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="55" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G55" s="4" t="s">
+    <row r="55" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G55" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="I55" s="6" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="57" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E58" t="s">
+    <row r="58" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="G58" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="I58" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G59" s="4" t="s">
+    <row r="59" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G59" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="I59" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="60" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G60" s="4" t="s">
+    <row r="60" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G60" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="I60" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="61" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G61" s="4" t="s">
+    <row r="61" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G61" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I61" s="4" t="s">
+      <c r="I61" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G62" s="4" t="s">
+    <row r="62" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G62" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I62" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G63" s="4" t="s">
+    <row r="63" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G63" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="I63" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G64" s="4" t="s">
+    <row r="64" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G64" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I64" s="4" t="s">
+      <c r="I64" s="6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G65" s="4" t="s">
+    <row r="65" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G65" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H65" t="s">
-        <v>32</v>
-      </c>
-      <c r="I65" s="4" t="s">
+      <c r="H65" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" s="6" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="66" spans="3:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="G66" s="4" t="s">
+    <row r="66" spans="3:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="G66" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="H66" t="s">
-        <v>32</v>
-      </c>
-      <c r="I66" s="4" t="s">
+      <c r="H66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I66" s="6" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="67" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G67" s="4" t="s">
+    <row r="67" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G67" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="I67" s="6" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="68" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G68" s="4" t="s">
+    <row r="68" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G68" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="H68" t="s">
-        <v>32</v>
-      </c>
-      <c r="I68" s="4" t="s">
+      <c r="H68" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I68" s="6" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="69" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G69" s="4" t="s">
+    <row r="69" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G69" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I69" s="4" t="s">
+      <c r="I69" s="6" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G72" s="4" t="s">
+    <row r="72" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G72" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I72" s="4" t="s">
+      <c r="I72" s="6" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="73" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G73" s="4" t="s">
+    <row r="73" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G73" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H73" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I73" s="4" t="s">
+      <c r="I73" s="6" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="76" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C76" s="3" t="s">
+    <row r="76" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C76" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G76" s="4" t="s">
+      <c r="G76" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I76" s="4" t="s">
+      <c r="I76" s="6" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="77" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
+    <row r="77" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="E77" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G77" s="4" t="s">
+      <c r="G77" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="H77" t="s">
-        <v>32</v>
-      </c>
-      <c r="I77" s="4" t="s">
+      <c r="H77" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I77" s="6" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="78" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
+    <row r="78" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E78" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G78" s="4" t="s">
+      <c r="G78" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H78" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I78" s="4" t="s">
+      <c r="I78" s="6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="79" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G79" s="4" t="s">
+    <row r="79" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G79" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H79" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I79" s="4" t="s">
+      <c r="I79" s="6" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="81" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C81" s="3" t="s">
+    <row r="81" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C81" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G81" s="4" t="s">
+      <c r="G81" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I81" s="4" t="s">
+      <c r="I81" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="82" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="E82" t="s">
+    <row r="82" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E82" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G82" s="4" t="s">
+      <c r="G82" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H82" t="s">
-        <v>32</v>
-      </c>
-      <c r="I82" s="4" t="s">
+      <c r="H82" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="83" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E83" t="s">
+    <row r="83" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E83" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G83" s="4" t="s">
+      <c r="G83" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I83" s="4" t="s">
+      <c r="I83" s="6" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G84" s="4" t="s">
+    <row r="84" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G84" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I84" s="4" t="s">
+      <c r="I84" s="6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="85" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G85" s="4" t="s">
+    <row r="85" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G85" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H85" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I85" s="4" t="s">
+      <c r="I85" s="6" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="87" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="C87" s="3" t="s">
+    <row r="87" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C87" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="G87" s="4" t="s">
+      <c r="G87" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H87" t="s">
+      <c r="H87" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I87" s="4" t="s">
+      <c r="I87" s="6" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="89" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C89" s="3" t="s">
+    <row r="89" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C89" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="G89" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H89" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="I89" s="6" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="90" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G90" s="4" t="s">
+    <row r="90" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G90" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H90" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I90" s="4" t="s">
+      <c r="I90" s="6" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="91" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G91" s="4" t="s">
+    <row r="91" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G91" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I91" s="4" t="s">
+      <c r="I91" s="6" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="92" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G92" s="4" t="s">
+    <row r="92" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G92" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H92" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I92" s="4" t="s">
+      <c r="I92" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="93" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G93" s="4" t="s">
+    <row r="93" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G93" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H93" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I93" s="4" t="s">
+      <c r="I93" s="6" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="94" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G94" s="4" t="s">
+    <row r="94" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G94" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H94" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="I94" s="4" t="s">
+      <c r="I94" s="6" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="97" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C97" s="3" t="s">
+    <row r="97" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C97" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G97" s="4" t="s">
+      <c r="G97" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H97" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I97" s="4" t="s">
+      <c r="I97" s="6" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="98" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="E98" t="s">
+    <row r="98" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E98" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G98" s="4" t="s">
+      <c r="G98" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H98" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="I98" s="6" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="99" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E99" t="s">
+    <row r="99" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E99" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G99" s="4" t="s">
+      <c r="G99" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H99" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I99" s="4" t="s">
+      <c r="I99" s="6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="102" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C102" s="3" t="s">
+    <row r="102" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C102" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G102" s="4" t="s">
+      <c r="G102" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H102" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="I102" s="4" t="s">
+      <c r="I102" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="103" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G103" s="4" t="s">
+    <row r="103" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G103" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H103" t="s">
-        <v>32</v>
-      </c>
-      <c r="I103" s="4" t="s">
+      <c r="H103" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I103" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="104" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G104" s="4" t="s">
+    <row r="104" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G104" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H104" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I104" s="4" t="s">
+      <c r="I104" s="6" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="107" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C107" s="3" t="s">
+    <row r="107" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C107" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G107" s="4" t="s">
+      <c r="G107" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H107" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="I107" s="4" t="s">
+      <c r="I107" s="6" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="110" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C110" s="3" t="s">
+    <row r="110" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C110" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="G110" s="4" t="s">
+      <c r="G110" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H110" t="s">
-        <v>32</v>
-      </c>
-      <c r="I110" s="4" t="s">
+      <c r="H110" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I110" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="111" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="G111" s="4" t="s">
+    <row r="111" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G111" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H111" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I111" s="4" t="s">
+      <c r="I111" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="114" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C114" s="3" t="s">
+    <row r="114" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C114" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G114" s="4" t="s">
+      <c r="G114" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="H114" t="s">
-        <v>32</v>
-      </c>
-      <c r="I114" s="4" t="s">
+      <c r="H114" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I114" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="115" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="G115" s="4" t="s">
+    <row r="115" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G115" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="H115" t="s">
-        <v>32</v>
-      </c>
-      <c r="I115" s="4" t="s">
+      <c r="H115" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I115" s="6" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="116" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G116" s="4" t="s">
+    <row r="116" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G116" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="H116" t="s">
-        <v>32</v>
-      </c>
-      <c r="I116" s="4" t="s">
+      <c r="H116" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I116" s="6" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="117" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G117" s="4" t="s">
+    <row r="117" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G117" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H117" t="s">
-        <v>32</v>
-      </c>
-      <c r="I117" s="4" t="s">
+      <c r="H117" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I117" s="6" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="118" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="G118" s="4" t="s">
+    <row r="118" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G118" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="H118" t="s">
-        <v>32</v>
-      </c>
-      <c r="I118" s="4" t="s">
+      <c r="H118" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I118" s="6" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="119" spans="3:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="G119" s="4" t="s">
+    <row r="119" spans="3:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="G119" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="H119" t="s">
+      <c r="H119" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="I119" s="4" t="s">
+      <c r="I119" s="6" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="3:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="G120" s="4" t="s">
+    <row r="120" spans="3:9" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="G120" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="H120" t="s">
-        <v>32</v>
-      </c>
-      <c r="I120" s="4" t="s">
+      <c r="H120" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I120" s="6" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="121" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G121" s="4" t="s">
+    <row r="121" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G121" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="H121" t="s">
+      <c r="H121" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="I121" s="4" t="s">
+      <c r="I121" s="6" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="122" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G122" s="4" t="s">
+      <c r="G122" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="H122" t="s">
+      <c r="H122" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="125" spans="3:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="C125" s="3" t="s">
+    <row r="125" spans="3:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C125" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D125" s="4" t="s">
+      <c r="D125" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="G125" s="4" t="s">
+      <c r="G125" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H125" t="s">
-        <v>32</v>
-      </c>
-      <c r="I125" s="4" t="s">
+      <c r="H125" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I125" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="126" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G126" s="4" t="s">
+    <row r="126" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G126" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="H126" t="s">
-        <v>32</v>
-      </c>
-      <c r="I126" s="4" t="s">
+      <c r="H126" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I126" s="6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="127" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G127" s="4" t="s">
+    <row r="127" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G127" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="H127" t="s">
-        <v>32</v>
-      </c>
-      <c r="I127" s="4" t="s">
+      <c r="H127" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I127" s="6" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="128" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="G128" s="4" t="s">
+    <row r="128" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G128" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="H128" t="s">
+      <c r="H128" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I128" s="4" t="s">
+      <c r="I128" s="6" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="129" spans="3:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="G129" s="4" t="s">
+    <row r="129" spans="3:9" ht="126" x14ac:dyDescent="0.25">
+      <c r="G129" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H129" t="s">
+      <c r="H129" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I129" s="4" t="s">
+      <c r="I129" s="6" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="130" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="G130" s="4" t="s">
+    <row r="130" spans="3:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G130" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="H130" t="s">
+      <c r="H130" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I130" s="4" t="s">
+      <c r="I130" s="6" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="133" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C133" s="3" t="s">
+    <row r="133" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C133" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G133" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I133" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="134" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="E134" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G134" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I134" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="135" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E135" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G135" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="I135" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="136" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E136" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G136" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I136" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="137" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G137" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I137" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="138" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G138" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I138" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="139" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+    </row>
+    <row r="141" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C141" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D141" s="6" t="s">
         <v>200</v>
+      </c>
+      <c r="G141" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I141" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="142" spans="3:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="G142" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="I142" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="143" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G143" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="I143" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="144" spans="3:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="G144" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I144" s="6" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>